<commit_message>
Hypothesis Test for Difference in Means Demo
Hypothesis Test for Difference in Means Demo - student-t pooled and unequal variance approaches.
</commit_message>
<xml_diff>
--- a/Difference_in_means_demo.xlsx
+++ b/Difference_in_means_demo.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>mean</t>
   </si>
@@ -218,6 +218,15 @@
   </si>
   <si>
     <t>The distribution of X1 and X2 is assumed to be Gaussian if the number of samples is small (&lt; 30).</t>
+  </si>
+  <si>
+    <t>dof</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -782,7 +791,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -926,6 +935,22 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1054,40 +1079,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="0.0">
-                  <c:v>-3.2588142900366717</c:v>
+                  <c:v>-3.7568783437819473</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.9551033802421554</c:v>
+                  <c:v>-3.408705914332002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.3476815606531227</c:v>
+                  <c:v>-2.7123610554321114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.7402597410640901</c:v>
+                  <c:v>-2.0160161965322208</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.1328379214750575</c:v>
+                  <c:v>-1.3196713376323301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.52541610188602483</c:v>
+                  <c:v>-0.62332647873243952</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2005717703007797E-2</c:v>
+                  <c:v>7.3018380167451102E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68942753729204043</c:v>
+                  <c:v>0.76936323906734172</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2968493568810731</c:v>
+                  <c:v>1.4657080979672323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9042711764701057</c:v>
+                  <c:v>2.162052956867123</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5116929960591383</c:v>
+                  <c:v>2.8583978157670136</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.0">
-                  <c:v>2.8154039058536546</c:v>
+                  <c:v>3.2065702452169584</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1102,37 +1127,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8571428571428571E-2</c:v>
+                  <c:v>9.5238095238095247E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8571428571428571E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5238095238095261E-2</c:v>
+                  <c:v>2.8571428571428574E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.12380952380952381</c:v>
+                  <c:v>0.14285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.18095238095238092</c:v>
+                  <c:v>0.19047619047619049</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.12380952380952387</c:v>
+                  <c:v>0.25714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.16190476190476188</c:v>
+                  <c:v>0.19047619047619047</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.16190476190476188</c:v>
+                  <c:v>0.1333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.7142857142857162E-2</c:v>
+                  <c:v>2.8571428571428581E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.8571428571428581E-2</c:v>
+                  <c:v>9.523809523809601E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-2.7210884353741507E-4</c:v>
+                  <c:v>-9.0702947845805722E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1178,40 +1203,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="0.0">
-                  <c:v>-3.5263532339540009</c:v>
+                  <c:v>-4.6131363481758925</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.1519242967566767</c:v>
+                  <c:v>-4.2182680862624728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.4030664223620279</c:v>
+                  <c:v>-3.4285315624356336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.6542085479673794</c:v>
+                  <c:v>-2.6387950386087944</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.9053506735727308</c:v>
+                  <c:v>-1.8490585147819549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.15649279917808223</c:v>
+                  <c:v>-1.0593219909551155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59236507521656634</c:v>
+                  <c:v>-0.26958546712827602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3412229496112149</c:v>
+                  <c:v>0.52015105669856343</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0900808240058635</c:v>
+                  <c:v>1.3098875805254029</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8389386984005123</c:v>
+                  <c:v>2.0996241043522423</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5877965727951606</c:v>
+                  <c:v>2.889360628179082</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9622255099924839</c:v>
+                  <c:v>3.2842288900925025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1226,34 +1251,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8095238095238099E-2</c:v>
+                  <c:v>2.8571428571428571E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>-1.9047619047619046E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.7619047619047616E-2</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13333333333333333</c:v>
+                  <c:v>1.9047619047619046E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.17142857142857143</c:v>
+                  <c:v>0.15238095238095237</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.11428571428571427</c:v>
+                  <c:v>0.14285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.28571428571428575</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18095238095238086</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.15238095238095239</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.20952380952380956</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.5714285714285632E-2</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.8095238095238182E-2</c:v>
+                  <c:v>3.8095238095238071E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0</c:v>
@@ -1695,40 +1720,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="0.0">
-                  <c:v>-3.2588142900366717</c:v>
+                  <c:v>-3.7568783437819473</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.9551033802421554</c:v>
+                  <c:v>-3.408705914332002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.3476815606531227</c:v>
+                  <c:v>-2.7123610554321114</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.7402597410640901</c:v>
+                  <c:v>-2.0160161965322208</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.1328379214750575</c:v>
+                  <c:v>-1.3196713376323301</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.52541610188602483</c:v>
+                  <c:v>-0.62332647873243952</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2005717703007797E-2</c:v>
+                  <c:v>7.3018380167451102E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68942753729204043</c:v>
+                  <c:v>0.76936323906734172</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.2968493568810731</c:v>
+                  <c:v>1.4657080979672323</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9042711764701057</c:v>
+                  <c:v>2.162052956867123</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.5116929960591383</c:v>
+                  <c:v>2.8583978157670136</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.0">
-                  <c:v>2.8154039058536546</c:v>
+                  <c:v>3.2065702452169584</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1743,31 +1768,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.8571428571428571E-2</c:v>
+                  <c:v>9.5238095238095247E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.7142857142857141E-2</c:v>
+                  <c:v>9.5238095238095247E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.15238095238095239</c:v>
+                  <c:v>3.8095238095238099E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27619047619047621</c:v>
+                  <c:v>0.18095238095238095</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45714285714285713</c:v>
+                  <c:v>0.37142857142857144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.580952380952381</c:v>
+                  <c:v>0.62857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.74285714285714288</c:v>
+                  <c:v>0.81904761904761902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.90476190476190477</c:v>
+                  <c:v>0.95238095238095233</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.96190476190476193</c:v>
+                  <c:v>0.98095238095238091</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.99047619047619051</c:v>
@@ -1819,40 +1844,40 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0" formatCode="0.0">
-                  <c:v>-3.5263532339540009</c:v>
+                  <c:v>-4.6131363481758925</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3.1519242967566767</c:v>
+                  <c:v>-4.2182680862624728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.4030664223620279</c:v>
+                  <c:v>-3.4285315624356336</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1.6542085479673794</c:v>
+                  <c:v>-2.6387950386087944</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.9053506735727308</c:v>
+                  <c:v>-1.8490585147819549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.15649279917808223</c:v>
+                  <c:v>-1.0593219909551155</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.59236507521656634</c:v>
+                  <c:v>-0.26958546712827602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3412229496112149</c:v>
+                  <c:v>0.52015105669856343</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0900808240058635</c:v>
+                  <c:v>1.3098875805254029</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8389386984005123</c:v>
+                  <c:v>2.0996241043522423</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.5877965727951606</c:v>
+                  <c:v>2.889360628179082</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.9622255099924839</c:v>
+                  <c:v>3.2842288900925025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1867,34 +1892,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.8095238095238099E-2</c:v>
+                  <c:v>2.8571428571428571E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8095238095238099E-2</c:v>
+                  <c:v>9.5238095238095247E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.5714285714285715E-2</c:v>
+                  <c:v>9.5238095238095247E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.21904761904761905</c:v>
+                  <c:v>2.8571428571428571E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.39047619047619048</c:v>
+                  <c:v>0.18095238095238095</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.50476190476190474</c:v>
+                  <c:v>0.32380952380952382</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.65714285714285714</c:v>
+                  <c:v>0.60952380952380958</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.8666666666666667</c:v>
+                  <c:v>0.79047619047619044</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.95238095238095233</c:v>
+                  <c:v>0.94285714285714284</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.99047619047619051</c:v>
+                  <c:v>0.98095238095238091</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>1</c:v>
@@ -3084,8 +3109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD150"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="X64" sqref="X64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3096,6 +3121,7 @@
     <col min="6" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="12.7109375" style="5" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="5"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.140625" customWidth="1"/>
     <col min="23" max="56" width="9.140625" style="1"/>
   </cols>
@@ -3394,43 +3420,43 @@
       </c>
       <c r="J9" s="7">
         <f ca="1">G11</f>
-        <v>-3.2588142900366717</v>
+        <v>-3.7568783437819473</v>
       </c>
       <c r="K9" s="8">
         <f t="shared" ref="K9:S9" ca="1" si="0">J9+($G$12-$G$11)/10</f>
-        <v>-2.651392470447639</v>
+        <v>-3.0605334848820567</v>
       </c>
       <c r="L9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>-2.0439706508586064</v>
+        <v>-2.3641886259821661</v>
       </c>
       <c r="M9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>-1.4365488312695738</v>
+        <v>-1.6678437670822754</v>
       </c>
       <c r="N9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.82912701168054115</v>
+        <v>-0.97149890818238482</v>
       </c>
       <c r="O9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>-0.22170519209150852</v>
+        <v>-0.27515404928249421</v>
       </c>
       <c r="P9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38571662749752411</v>
+        <v>0.42119080961739641</v>
       </c>
       <c r="Q9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99313844708655674</v>
+        <v>1.117535668517287</v>
       </c>
       <c r="R9" s="8">
         <f t="shared" ca="1" si="0"/>
-        <v>1.6005602666755894</v>
+        <v>1.8138805274171776</v>
       </c>
       <c r="S9" s="9">
         <f t="shared" ca="1" si="0"/>
-        <v>2.207982086264622</v>
+        <v>2.5102253863170683</v>
       </c>
       <c r="T9" s="28"/>
       <c r="U9" s="28"/>
@@ -3451,43 +3477,43 @@
       <c r="I10" s="66"/>
       <c r="J10" s="10">
         <f t="shared" ref="J10:S10" ca="1" si="1">J9+($G$12-$G$11)/10</f>
-        <v>-2.651392470447639</v>
+        <v>-3.0605334848820567</v>
       </c>
       <c r="K10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.0439706508586064</v>
+        <v>-2.3641886259821661</v>
       </c>
       <c r="L10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.4365488312695738</v>
+        <v>-1.6678437670822754</v>
       </c>
       <c r="M10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.82912701168054115</v>
+        <v>-0.97149890818238482</v>
       </c>
       <c r="N10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.22170519209150852</v>
+        <v>-0.27515404928249421</v>
       </c>
       <c r="O10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.38571662749752411</v>
+        <v>0.42119080961739641</v>
       </c>
       <c r="P10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>0.99313844708655674</v>
+        <v>1.117535668517287</v>
       </c>
       <c r="Q10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>1.6005602666755894</v>
+        <v>1.8138805274171776</v>
       </c>
       <c r="R10" s="11">
         <f t="shared" ca="1" si="1"/>
-        <v>2.207982086264622</v>
+        <v>2.5102253863170683</v>
       </c>
       <c r="S10" s="12">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8154039058536546</v>
+        <v>3.2065702452169589</v>
       </c>
       <c r="T10" s="28"/>
       <c r="U10" s="28"/>
@@ -3509,58 +3535,58 @@
       </c>
       <c r="G11" s="13">
         <f ca="1">MIN(C20:C124)</f>
-        <v>-3.2588142900366717</v>
+        <v>-3.7568783437819473</v>
       </c>
       <c r="H11" s="32" t="s">
         <v>2</v>
       </c>
       <c r="I11" s="21">
         <f ca="1">G11</f>
-        <v>-3.2588142900366717</v>
+        <v>-3.7568783437819473</v>
       </c>
       <c r="J11" s="8">
         <f ca="1">$G$11+($G$12-$G$11)/20</f>
-        <v>-2.9551033802421554</v>
+        <v>-3.408705914332002</v>
       </c>
       <c r="K11" s="8">
         <f t="shared" ref="K11:S11" ca="1" si="2">J11+($G$12-$G$11)/10</f>
-        <v>-2.3476815606531227</v>
+        <v>-2.7123610554321114</v>
       </c>
       <c r="L11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.7402597410640901</v>
+        <v>-2.0160161965322208</v>
       </c>
       <c r="M11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>-1.1328379214750575</v>
+        <v>-1.3196713376323301</v>
       </c>
       <c r="N11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.52541610188602483</v>
+        <v>-0.62332647873243952</v>
       </c>
       <c r="O11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>8.2005717703007797E-2</v>
+        <v>7.3018380167451102E-2</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>0.68942753729204043</v>
+        <v>0.76936323906734172</v>
       </c>
       <c r="Q11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1.2968493568810731</v>
+        <v>1.4657080979672323</v>
       </c>
       <c r="R11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1.9042711764701057</v>
+        <v>2.162052956867123</v>
       </c>
       <c r="S11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2.5116929960591383</v>
+        <v>2.8583978157670136</v>
       </c>
       <c r="T11" s="15">
         <f ca="1">G12</f>
-        <v>2.8154039058536546</v>
+        <v>3.2065702452169584</v>
       </c>
       <c r="U11" s="28"/>
       <c r="V11" s="31"/>
@@ -3581,7 +3607,7 @@
       </c>
       <c r="G12" s="14">
         <f ca="1">MAX(C20:C124)</f>
-        <v>2.8154039058536546</v>
+        <v>3.2065702452169584</v>
       </c>
       <c r="H12" s="32" t="s">
         <v>6</v>
@@ -3591,47 +3617,47 @@
       </c>
       <c r="J12" s="11">
         <f ca="1">COUNTIF($C$20:$C$124,"&lt;"&amp;J10)/COUNT($C$20:$C$124)</f>
-        <v>2.8571428571428571E-2</v>
+        <v>9.5238095238095247E-3</v>
       </c>
       <c r="K12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;K10))/COUNT($C$20:$C$124)-J12</f>
-        <v>2.8571428571428571E-2</v>
+        <v>0</v>
       </c>
       <c r="L12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;L10))/COUNT($C$20:$C$124)-SUM($J$12:K12)</f>
-        <v>9.5238095238095261E-2</v>
+        <v>2.8571428571428574E-2</v>
       </c>
       <c r="M12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;M10))/COUNT($C$20:$C$124)-SUM($J$12:L12)</f>
-        <v>0.12380952380952381</v>
+        <v>0.14285714285714285</v>
       </c>
       <c r="N12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;N10))/COUNT($C$20:$C$124)-SUM($J$12:M12)</f>
-        <v>0.18095238095238092</v>
+        <v>0.19047619047619049</v>
       </c>
       <c r="O12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;O10))/COUNT($C$20:$C$124)-SUM($J$12:N12)</f>
-        <v>0.12380952380952387</v>
+        <v>0.25714285714285712</v>
       </c>
       <c r="P12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;P10))/COUNT($C$20:$C$124)-SUM($J$12:O12)</f>
-        <v>0.16190476190476188</v>
+        <v>0.19047619047619047</v>
       </c>
       <c r="Q12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;Q10))/COUNT($C$20:$C$124)-SUM($J$12:P12)</f>
-        <v>0.16190476190476188</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="R12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;R10))/COUNT($C$20:$C$124)-SUM($J$12:Q12)</f>
-        <v>5.7142857142857162E-2</v>
+        <v>2.8571428571428581E-2</v>
       </c>
       <c r="S12" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;S10))/COUNT($C$20:$C$124)-SUM($J$12:R12)</f>
-        <v>2.8571428571428581E-2</v>
+        <v>9.523809523809601E-3</v>
       </c>
       <c r="T12" s="12">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;T10)-S12)/COUNT($C$20:$C$124)</f>
-        <v>-2.7210884353741507E-4</v>
+        <v>-9.0702947845805722E-5</v>
       </c>
       <c r="U12" s="28"/>
       <c r="V12" s="31"/>
@@ -3655,39 +3681,39 @@
       </c>
       <c r="J13" s="19">
         <f t="shared" ref="J13:S13" ca="1" si="3">J12+I13</f>
-        <v>2.8571428571428571E-2</v>
+        <v>9.5238095238095247E-3</v>
       </c>
       <c r="K13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>5.7142857142857141E-2</v>
+        <v>9.5238095238095247E-3</v>
       </c>
       <c r="L13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.15238095238095239</v>
+        <v>3.8095238095238099E-2</v>
       </c>
       <c r="M13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.27619047619047621</v>
+        <v>0.18095238095238095</v>
       </c>
       <c r="N13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.45714285714285713</v>
+        <v>0.37142857142857144</v>
       </c>
       <c r="O13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.580952380952381</v>
+        <v>0.62857142857142856</v>
       </c>
       <c r="P13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.74285714285714288</v>
+        <v>0.81904761904761902</v>
       </c>
       <c r="Q13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.90476190476190477</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="R13" s="19">
         <f t="shared" ca="1" si="3"/>
-        <v>0.96190476190476193</v>
+        <v>0.98095238095238091</v>
       </c>
       <c r="S13" s="19">
         <f t="shared" ca="1" si="3"/>
@@ -3813,43 +3839,43 @@
       </c>
       <c r="J15" s="7">
         <f ca="1">G17</f>
-        <v>-3.5263532339540009</v>
+        <v>-4.6131363481758925</v>
       </c>
       <c r="K15" s="8">
         <f t="shared" ref="K15:S15" ca="1" si="4">J15+($G$12-$G$11)/10</f>
-        <v>-2.9189314143649683</v>
+        <v>-3.9167914892760018</v>
       </c>
       <c r="L15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.3115095947759356</v>
+        <v>-3.2204466303761112</v>
       </c>
       <c r="M15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.704087775186903</v>
+        <v>-2.5241017714762206</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>-1.0966659555978704</v>
+        <v>-1.82775691257633</v>
       </c>
       <c r="O15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>-0.48924413600883776</v>
+        <v>-1.1314120536764394</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.11817768358019487</v>
+        <v>-0.43506719477654876</v>
       </c>
       <c r="Q15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>0.7255995031692275</v>
+        <v>0.26127766412334186</v>
       </c>
       <c r="R15" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>1.3330213227582601</v>
+        <v>0.95762252302323247</v>
       </c>
       <c r="S15" s="9">
         <f t="shared" ca="1" si="4"/>
-        <v>1.9404431423472928</v>
+        <v>1.6539673819231231</v>
       </c>
       <c r="T15" s="28"/>
       <c r="U15" s="28"/>
@@ -3905,43 +3931,43 @@
       <c r="I16" s="66"/>
       <c r="J16" s="10">
         <f t="shared" ref="J16:S16" ca="1" si="5">J15+($G$12-$G$11)/10</f>
-        <v>-2.9189314143649683</v>
+        <v>-3.9167914892760018</v>
       </c>
       <c r="K16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>-2.3115095947759356</v>
+        <v>-3.2204466303761112</v>
       </c>
       <c r="L16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>-1.704087775186903</v>
+        <v>-2.5241017714762206</v>
       </c>
       <c r="M16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>-1.0966659555978704</v>
+        <v>-1.82775691257633</v>
       </c>
       <c r="N16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>-0.48924413600883776</v>
+        <v>-1.1314120536764394</v>
       </c>
       <c r="O16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>0.11817768358019487</v>
+        <v>-0.43506719477654876</v>
       </c>
       <c r="P16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>0.7255995031692275</v>
+        <v>0.26127766412334186</v>
       </c>
       <c r="Q16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>1.3330213227582601</v>
+        <v>0.95762252302323247</v>
       </c>
       <c r="R16" s="11">
         <f t="shared" ca="1" si="5"/>
-        <v>1.9404431423472928</v>
+        <v>1.6539673819231231</v>
       </c>
       <c r="S16" s="12">
         <f t="shared" ca="1" si="5"/>
-        <v>2.5478649619363254</v>
+        <v>2.3503122408230137</v>
       </c>
       <c r="T16" s="28"/>
       <c r="U16" s="28"/>
@@ -3992,58 +4018,58 @@
       </c>
       <c r="G17" s="13">
         <f ca="1">MIN(D20:D124)</f>
-        <v>-3.5263532339540009</v>
+        <v>-4.6131363481758925</v>
       </c>
       <c r="H17" s="32" t="s">
         <v>3</v>
       </c>
       <c r="I17" s="21">
         <f ca="1">G17</f>
-        <v>-3.5263532339540009</v>
+        <v>-4.6131363481758925</v>
       </c>
       <c r="J17" s="8">
         <f ca="1">$G$17+($G$18-$G$17)/20</f>
-        <v>-3.1519242967566767</v>
+        <v>-4.2182680862624728</v>
       </c>
       <c r="K17" s="8">
         <f ca="1">J17+($G$18-$G$17)/10</f>
-        <v>-2.4030664223620279</v>
+        <v>-3.4285315624356336</v>
       </c>
       <c r="L17" s="8">
         <f t="shared" ref="L17:S17" ca="1" si="6">K17+($G$18-$G$17)/10</f>
-        <v>-1.6542085479673794</v>
+        <v>-2.6387950386087944</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.9053506735727308</v>
+        <v>-1.8490585147819549</v>
       </c>
       <c r="N17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>-0.15649279917808223</v>
+        <v>-1.0593219909551155</v>
       </c>
       <c r="O17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>0.59236507521656634</v>
+        <v>-0.26958546712827602</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>1.3412229496112149</v>
+        <v>0.52015105669856343</v>
       </c>
       <c r="Q17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>2.0900808240058635</v>
+        <v>1.3098875805254029</v>
       </c>
       <c r="R17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>2.8389386984005123</v>
+        <v>2.0996241043522423</v>
       </c>
       <c r="S17" s="8">
         <f t="shared" ca="1" si="6"/>
-        <v>3.5877965727951606</v>
+        <v>2.889360628179082</v>
       </c>
       <c r="T17" s="9">
         <f ca="1">G18</f>
-        <v>3.9622255099924839</v>
+        <v>3.2842288900925025</v>
       </c>
       <c r="U17" s="28"/>
       <c r="V17" s="29"/>
@@ -4095,7 +4121,7 @@
       </c>
       <c r="G18" s="14">
         <f ca="1">MAX(D20:D124)</f>
-        <v>3.9622255099924839</v>
+        <v>3.2842288900925025</v>
       </c>
       <c r="H18" s="32" t="s">
         <v>6</v>
@@ -4105,43 +4131,43 @@
       </c>
       <c r="J18" s="11">
         <f ca="1">COUNTIF($D$20:$D$124,"&lt;"&amp;J16)/COUNT($D$20:$D$124)</f>
-        <v>3.8095238095238099E-2</v>
+        <v>2.8571428571428571E-2</v>
       </c>
       <c r="K18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;K16))/COUNT($C$20:$C$124)-J18</f>
-        <v>0</v>
+        <v>-1.9047619047619046E-2</v>
       </c>
       <c r="L18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;L16))/COUNT($C$20:$C$124)-SUM($J$18:K18)</f>
-        <v>4.7619047619047616E-2</v>
+        <v>0</v>
       </c>
       <c r="M18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;M16))/COUNT($C$20:$C$124)-SUM($J$18:L18)</f>
-        <v>0.13333333333333333</v>
+        <v>1.9047619047619046E-2</v>
       </c>
       <c r="N18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;N16))/COUNT($C$20:$C$124)-SUM($J$18:M18)</f>
-        <v>0.17142857142857143</v>
+        <v>0.15238095238095237</v>
       </c>
       <c r="O18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;O16))/COUNT($C$20:$C$124)-SUM($J$18:N18)</f>
-        <v>0.11428571428571427</v>
+        <v>0.14285714285714288</v>
       </c>
       <c r="P18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;P16))/COUNT($C$20:$C$124)-SUM($J$18:O18)</f>
-        <v>0.15238095238095239</v>
+        <v>0.28571428571428575</v>
       </c>
       <c r="Q18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;Q16))/COUNT($C$20:$C$124)-SUM($J$18:P18)</f>
-        <v>0.20952380952380956</v>
+        <v>0.18095238095238086</v>
       </c>
       <c r="R18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;R16))/COUNT($C$20:$C$124)-SUM($J$18:Q18)</f>
-        <v>8.5714285714285632E-2</v>
+        <v>0.15238095238095239</v>
       </c>
       <c r="S18" s="11">
         <f ca="1">(COUNTIF($C$20:$C$124,"&lt;"&amp;S16))/COUNT($C$20:$C$124)-SUM($J$18:R18)</f>
-        <v>3.8095238095238182E-2</v>
+        <v>3.8095238095238071E-2</v>
       </c>
       <c r="T18" s="12">
         <v>0</v>
@@ -4204,43 +4230,43 @@
       </c>
       <c r="J19" s="19">
         <f t="shared" ref="J19:S19" ca="1" si="7">J18+I19</f>
-        <v>3.8095238095238099E-2</v>
+        <v>2.8571428571428571E-2</v>
       </c>
       <c r="K19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>3.8095238095238099E-2</v>
+        <v>9.5238095238095247E-3</v>
       </c>
       <c r="L19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>8.5714285714285715E-2</v>
+        <v>9.5238095238095247E-3</v>
       </c>
       <c r="M19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.21904761904761905</v>
+        <v>2.8571428571428571E-2</v>
       </c>
       <c r="N19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.39047619047619048</v>
+        <v>0.18095238095238095</v>
       </c>
       <c r="O19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.50476190476190474</v>
+        <v>0.32380952380952382</v>
       </c>
       <c r="P19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.65714285714285714</v>
+        <v>0.60952380952380958</v>
       </c>
       <c r="Q19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.8666666666666667</v>
+        <v>0.79047619047619044</v>
       </c>
       <c r="R19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.95238095238095233</v>
+        <v>0.94285714285714284</v>
       </c>
       <c r="S19" s="19">
         <f t="shared" ca="1" si="7"/>
-        <v>0.99047619047619051</v>
+        <v>0.98095238095238091</v>
       </c>
       <c r="T19" s="20">
         <v>1</v>
@@ -4287,11 +4313,11 @@
       <c r="B20" s="27"/>
       <c r="C20" s="36">
         <f t="shared" ref="C20:C51" ca="1" si="8">_xlfn.NORM.INV(RAND(),$D$11,$D$12)</f>
-        <v>-0.22397052107949306</v>
+        <v>-1.2750285884858339</v>
       </c>
       <c r="D20" s="36">
         <f t="shared" ref="D20:D51" ca="1" si="9">_xlfn.NORM.INV(RAND(),$D$15,$D$16)</f>
-        <v>-0.8636677186174615</v>
+        <v>1.610727367355776</v>
       </c>
       <c r="E20" s="36"/>
       <c r="F20" s="28"/>
@@ -4351,11 +4377,11 @@
       <c r="B21" s="27"/>
       <c r="C21" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1205714336318044</v>
+        <v>-0.17483151319947715</v>
       </c>
       <c r="D21" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-3.340774864018023</v>
+        <v>1.2046622505832403</v>
       </c>
       <c r="E21" s="36"/>
       <c r="F21" s="28"/>
@@ -4415,11 +4441,11 @@
       <c r="B22" s="27"/>
       <c r="C22" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5788789352814998</v>
+        <v>-2.2130705699166406</v>
       </c>
       <c r="D22" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.53330176984897648</v>
+        <v>-3.9838874979253953</v>
       </c>
       <c r="E22" s="36"/>
       <c r="F22" s="28"/>
@@ -4479,11 +4505,11 @@
       <c r="B23" s="27"/>
       <c r="C23" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>0.4559996799187625</v>
+        <v>-4.9972375940542449E-2</v>
       </c>
       <c r="D23" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.4074792980859343</v>
+        <v>0.43262977975485983</v>
       </c>
       <c r="E23" s="36"/>
       <c r="F23" s="28"/>
@@ -4543,11 +4569,11 @@
       <c r="B24" s="27"/>
       <c r="C24" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.43550932767601963</v>
+        <v>-1.1638591814296204</v>
       </c>
       <c r="D24" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.413267406296286</v>
+        <v>-2.4866286202051997</v>
       </c>
       <c r="E24" s="36"/>
       <c r="F24" s="28"/>
@@ -4607,11 +4633,11 @@
       <c r="B25" s="27"/>
       <c r="C25" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.2581654978997614</v>
+        <v>-8.7687319419761253E-2</v>
       </c>
       <c r="D25" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.66219425210145899</v>
+        <v>-2.2007513137469137</v>
       </c>
       <c r="E25" s="36"/>
       <c r="F25" s="28"/>
@@ -4671,11 +4697,11 @@
       <c r="B26" s="27"/>
       <c r="C26" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>0.67987872242967851</v>
+        <v>-1.2109469147025276</v>
       </c>
       <c r="D26" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>1.5641274358195425</v>
+        <v>1.0865381714977747</v>
       </c>
       <c r="E26" s="36"/>
       <c r="F26" s="28"/>
@@ -4735,11 +4761,11 @@
       <c r="B27" s="27"/>
       <c r="C27" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.5880952723774024</v>
+        <v>1.2213926253348377</v>
       </c>
       <c r="D27" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.28285963801410291</v>
+        <v>3.1510830276016666</v>
       </c>
       <c r="E27" s="36"/>
       <c r="F27" s="28"/>
@@ -4799,11 +4825,11 @@
       <c r="B28" s="27"/>
       <c r="C28" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1896978752612328</v>
+        <v>-8.7764978669684954E-2</v>
       </c>
       <c r="D28" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>1.4934099579771598E-2</v>
+        <v>-4.2164407867677669</v>
       </c>
       <c r="E28" s="36"/>
       <c r="F28" s="28"/>
@@ -4863,11 +4889,11 @@
       <c r="B29" s="27"/>
       <c r="C29" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1010695825460683</v>
+        <v>5.5903457378726144E-2</v>
       </c>
       <c r="D29" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.33952848371372246</v>
+        <v>-1.3052161928637918</v>
       </c>
       <c r="E29" s="36"/>
       <c r="F29" s="28"/>
@@ -4927,11 +4953,11 @@
       <c r="B30" s="27"/>
       <c r="C30" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.4093589394398035</v>
+        <v>0.10787051695312756</v>
       </c>
       <c r="D30" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.72752172267027726</v>
+        <v>-0.53674496969713292</v>
       </c>
       <c r="E30" s="36"/>
       <c r="F30" s="28"/>
@@ -4991,11 +5017,11 @@
       <c r="B31" s="27"/>
       <c r="C31" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>0.12919898367914678</v>
+        <v>-0.59481669861597763</v>
       </c>
       <c r="D31" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.1821053466364095</v>
+        <v>-0.1413502505319218</v>
       </c>
       <c r="E31" s="36"/>
       <c r="F31" s="28"/>
@@ -5055,11 +5081,11 @@
       <c r="B32" s="27"/>
       <c r="C32" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.7740571256083273</v>
+        <v>-2.231157920747012</v>
       </c>
       <c r="D32" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.8365799019357976</v>
+        <v>0.74844017477618396</v>
       </c>
       <c r="E32" s="36"/>
       <c r="F32" s="28"/>
@@ -5119,11 +5145,11 @@
       <c r="B33" s="27"/>
       <c r="C33" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2418141310028346</v>
+        <v>0.56861258303018924</v>
       </c>
       <c r="D33" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.61588097879165915</v>
+        <v>-2.7309832129201723</v>
       </c>
       <c r="E33" s="36"/>
       <c r="F33" s="28"/>
@@ -5183,11 +5209,11 @@
       <c r="B34" s="27"/>
       <c r="C34" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.3454781226119397</v>
+        <v>-0.83056486227240056</v>
       </c>
       <c r="D34" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.54969970328979412</v>
+        <v>-0.81152283306054596</v>
       </c>
       <c r="E34" s="36"/>
       <c r="F34" s="28"/>
@@ -5247,11 +5273,11 @@
       <c r="B35" s="27"/>
       <c r="C35" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2407843594580961</v>
+        <v>0.76396278445783228</v>
       </c>
       <c r="D35" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.2415805668662658</v>
+        <v>-1.1198039166428624</v>
       </c>
       <c r="E35" s="36"/>
       <c r="F35" s="28"/>
@@ -5311,11 +5337,11 @@
       <c r="B36" s="27"/>
       <c r="C36" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.0610729895639837E-2</v>
+        <v>0.85091211674002787</v>
       </c>
       <c r="D36" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.54900914523656641</v>
+        <v>0.43778615409276017</v>
       </c>
       <c r="E36" s="36"/>
       <c r="F36" s="28"/>
@@ -5375,11 +5401,11 @@
       <c r="B37" s="27"/>
       <c r="C37" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.8001644546902662</v>
+        <v>0.75390608966636763</v>
       </c>
       <c r="D37" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.47217457657212314</v>
+        <v>1.9562759238344776</v>
       </c>
       <c r="E37" s="36"/>
       <c r="F37" s="28"/>
@@ -5439,11 +5465,11 @@
       <c r="B38" s="27"/>
       <c r="C38" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5449356416175399</v>
+        <v>-1.1715441176442856</v>
       </c>
       <c r="D38" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.41937686023255194</v>
+        <v>0.22764455592167285</v>
       </c>
       <c r="E38" s="36"/>
       <c r="F38" s="56" t="s">
@@ -5505,11 +5531,11 @@
       <c r="B39" s="27"/>
       <c r="C39" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>0.94432865451449222</v>
+        <v>-0.12823569607265423</v>
       </c>
       <c r="D39" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-5.2319565288769701E-2</v>
+        <v>-6.7984542630575545E-2</v>
       </c>
       <c r="E39" s="36"/>
       <c r="F39" s="28"/>
@@ -5569,11 +5595,11 @@
       <c r="B40" s="27"/>
       <c r="C40" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.6110625834786265</v>
+        <v>1.4364178051426246</v>
       </c>
       <c r="D40" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.2294413581278989</v>
+        <v>1.8910862108095648E-2</v>
       </c>
       <c r="E40" s="36"/>
       <c r="F40" s="52" t="s">
@@ -5639,11 +5665,11 @@
       <c r="B41" s="27"/>
       <c r="C41" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.4481888549564488</v>
+        <v>-1.4235386473603797</v>
       </c>
       <c r="D41" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>1.2119931209810602</v>
+        <v>-1.5120052640603623</v>
       </c>
       <c r="E41" s="36"/>
       <c r="F41" s="28"/>
@@ -5703,11 +5729,11 @@
       <c r="B42" s="27"/>
       <c r="C42" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>2.8154039058536546</v>
+        <v>-1.15959344107741</v>
       </c>
       <c r="D42" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>9.0718525301147199E-2</v>
+        <v>0.16385187128548195</v>
       </c>
       <c r="E42" s="36"/>
       <c r="F42" s="44" t="s">
@@ -5723,7 +5749,7 @@
       <c r="L42" s="28"/>
       <c r="M42" s="46">
         <f ca="1">ABS(G43-G48)</f>
-        <v>0.16217814826438878</v>
+        <v>0.24812140399596552</v>
       </c>
       <c r="N42" s="28"/>
       <c r="O42" s="28"/>
@@ -5780,11 +5806,11 @@
       <c r="B43" s="27"/>
       <c r="C43" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>0.11539626530738033</v>
+        <v>1.120536038050866</v>
       </c>
       <c r="D43" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>1.7941618772083174</v>
+        <v>0.69703984396661267</v>
       </c>
       <c r="E43" s="36"/>
       <c r="F43" s="32" t="s">
@@ -5792,7 +5818,7 @@
       </c>
       <c r="G43" s="51">
         <f ca="1">AVERAGE(XOne)</f>
-        <v>-1.5552308157788439E-2</v>
+        <v>4.5842519653372264E-2</v>
       </c>
       <c r="H43" s="28"/>
       <c r="I43" s="28"/>
@@ -5803,7 +5829,7 @@
       <c r="L43" s="28"/>
       <c r="M43" s="47">
         <f ca="1">SQRT((1/G45+1/G50)*(((G45-1)*G44^2+(G50-1)*G49^2)/(G45+G50-2)))</f>
-        <v>0.19179016621122028</v>
+        <v>0.1888092019902069</v>
       </c>
       <c r="N43" s="28"/>
       <c r="O43" s="28"/>
@@ -5817,7 +5843,7 @@
       </c>
       <c r="S43" s="50">
         <f ca="1">M45</f>
-        <v>0.84560200070831837</v>
+        <v>1.3141383014204733</v>
       </c>
       <c r="T43" s="34" t="s">
         <v>20</v>
@@ -5867,11 +5893,11 @@
       <c r="B44" s="27"/>
       <c r="C44" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.5488571392409636</v>
+        <v>0.88463503191277548</v>
       </c>
       <c r="D44" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.8472040313959162</v>
+        <v>-0.71243066241454112</v>
       </c>
       <c r="E44" s="36"/>
       <c r="F44" s="32" t="s">
@@ -5879,7 +5905,7 @@
       </c>
       <c r="G44" s="51">
         <f ca="1">_xlfn.STDEV.S(XOne)</f>
-        <v>1.2899407616014686</v>
+        <v>1.1298032396516007</v>
       </c>
       <c r="H44" s="28"/>
       <c r="I44" s="28"/>
@@ -5936,11 +5962,11 @@
       <c r="B45" s="27"/>
       <c r="C45" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.0200920356230567</v>
+        <v>0.15373569961820782</v>
       </c>
       <c r="D45" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>1.6137301261179506</v>
+        <v>-1.3682517122949638</v>
       </c>
       <c r="E45" s="36"/>
       <c r="F45" s="32" t="s">
@@ -5959,7 +5985,7 @@
       <c r="L45" s="28"/>
       <c r="M45" s="46">
         <f ca="1">M42/M43</f>
-        <v>0.84560200070831837</v>
+        <v>1.3141383014204733</v>
       </c>
       <c r="N45" s="28"/>
       <c r="O45" s="28"/>
@@ -6013,11 +6039,11 @@
       <c r="B46" s="27"/>
       <c r="C46" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.7472037622711909</v>
+        <v>0.56249343584835154</v>
       </c>
       <c r="D46" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-1.5402332172160986</v>
+        <v>2.6052266889734472</v>
       </c>
       <c r="E46" s="36"/>
       <c r="F46" s="28"/>
@@ -6082,11 +6108,11 @@
       <c r="B47" s="27"/>
       <c r="C47" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-1.2827400268660387</v>
+        <v>1.191773638980266</v>
       </c>
       <c r="D47" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>-0.91659759494094994</v>
+        <v>0.81947718730621966</v>
       </c>
       <c r="E47" s="36"/>
       <c r="F47" s="44" t="s">
@@ -6148,11 +6174,11 @@
       <c r="B48" s="27"/>
       <c r="C48" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>1.1735965419317946</v>
+        <v>-0.60233900251477945</v>
       </c>
       <c r="D48" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.322209135246454</v>
+        <v>-0.93332537437123309</v>
       </c>
       <c r="E48" s="36"/>
       <c r="F48" s="32" t="s">
@@ -6160,7 +6186,7 @@
       </c>
       <c r="G48" s="46">
         <f ca="1">AVERAGE(XTwo)</f>
-        <v>-0.17773045642217722</v>
+        <v>-0.20227888434259325</v>
       </c>
       <c r="H48" s="28"/>
       <c r="I48" s="28"/>
@@ -6217,11 +6243,11 @@
       <c r="B49" s="27"/>
       <c r="C49" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-7.5183964224927805E-2</v>
+        <v>3.1722182313540515E-2</v>
       </c>
       <c r="D49" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>0.1559742083504283</v>
+        <v>2.1173052223481883</v>
       </c>
       <c r="E49" s="36"/>
       <c r="F49" s="32" t="s">
@@ -6229,7 +6255,7 @@
       </c>
       <c r="G49" s="51">
         <f ca="1">_xlfn.STDEV.S(XTwo)</f>
-        <v>1.4826722349758932</v>
+        <v>1.5705669960468149</v>
       </c>
       <c r="H49" s="28"/>
       <c r="I49" s="28"/>
@@ -6286,11 +6312,11 @@
       <c r="B50" s="27"/>
       <c r="C50" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>-0.95501008466461279</v>
+        <v>1.3736587038970187</v>
       </c>
       <c r="D50" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>2.2667988622673056</v>
+        <v>-1.5285917083489311</v>
       </c>
       <c r="E50" s="36"/>
       <c r="F50" s="32" t="s">
@@ -6355,11 +6381,11 @@
       <c r="B51" s="27"/>
       <c r="C51" s="36">
         <f t="shared" ca="1" si="8"/>
-        <v>0.77418010638396839</v>
+        <v>2.0997981498164031</v>
       </c>
       <c r="D51" s="36">
         <f t="shared" ca="1" si="9"/>
-        <v>1.8113384992254646</v>
+        <v>-0.39950804411832364</v>
       </c>
       <c r="E51" s="36"/>
       <c r="F51" s="28"/>
@@ -6419,11 +6445,11 @@
       <c r="B52" s="27"/>
       <c r="C52" s="36">
         <f t="shared" ref="C52:C83" ca="1" si="10">_xlfn.NORM.INV(RAND(),$D$11,$D$12)</f>
-        <v>0.43231284282537108</v>
+        <v>-1.2691131352251579</v>
       </c>
       <c r="D52" s="36">
         <f t="shared" ref="D52:D83" ca="1" si="11">_xlfn.NORM.INV(RAND(),$D$15,$D$16)</f>
-        <v>0.76947913964385251</v>
+        <v>0.36884353780242241</v>
       </c>
       <c r="E52" s="36"/>
       <c r="F52" s="28"/>
@@ -6483,11 +6509,11 @@
       <c r="B53" s="27"/>
       <c r="C53" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>2.4025991367324549E-2</v>
+        <v>-0.93905039775304056</v>
       </c>
       <c r="D53" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>0.2212031140208246</v>
+        <v>0.42070794023311842</v>
       </c>
       <c r="E53" s="36"/>
       <c r="F53" s="55" t="s">
@@ -6551,11 +6577,11 @@
       <c r="B54" s="27"/>
       <c r="C54" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.5957648348394009</v>
+        <v>-0.53788438279490336</v>
       </c>
       <c r="D54" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>0.75280759706616807</v>
+        <v>0.8020990256355025</v>
       </c>
       <c r="E54" s="36"/>
       <c r="F54" s="28"/>
@@ -6615,11 +6641,11 @@
       <c r="B55" s="27"/>
       <c r="C55" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.24527247265489494</v>
+        <v>1.786866302227305</v>
       </c>
       <c r="D55" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.071306830305703</v>
+        <v>-1.9332517378469183</v>
       </c>
       <c r="E55" s="36"/>
       <c r="F55" s="28" t="s">
@@ -6642,7 +6668,7 @@
       </c>
       <c r="R55" s="57">
         <f ca="1">_xlfn.T.DIST.2T(S43,(G45+G50-2))</f>
-        <v>0.39874649903910708</v>
+        <v>0.19024706136076203</v>
       </c>
       <c r="S55" s="49"/>
       <c r="T55" s="30"/>
@@ -6688,11 +6714,11 @@
       <c r="B56" s="27"/>
       <c r="C56" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.55520656095283605</v>
+        <v>-0.8997187904883186</v>
       </c>
       <c r="D56" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>0.98779799968111215</v>
+        <v>-1.6838378382763288</v>
       </c>
       <c r="E56" s="36"/>
       <c r="F56" s="28"/>
@@ -6752,11 +6778,11 @@
       <c r="B57" s="27"/>
       <c r="C57" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-3.2588142900366717</v>
+        <v>-0.74270905935348741</v>
       </c>
       <c r="D57" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>1.8043897748235587</v>
+        <v>1.4418761334040793</v>
       </c>
       <c r="E57" s="36"/>
       <c r="F57" s="28"/>
@@ -6816,11 +6842,11 @@
       <c r="B58" s="27"/>
       <c r="C58" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>1.5561734719832205</v>
+        <v>0.53651273056669413</v>
       </c>
       <c r="D58" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-0.53829933886565762</v>
+        <v>2.0789394755000985E-2</v>
       </c>
       <c r="E58" s="36"/>
       <c r="F58" s="58"/>
@@ -6880,11 +6906,11 @@
       <c r="B59" s="27"/>
       <c r="C59" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.32527313213818199</v>
+        <v>1.0041172408566619</v>
       </c>
       <c r="D59" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.3814983136809362</v>
+        <v>2.5766952363373692</v>
       </c>
       <c r="E59" s="36"/>
       <c r="F59" s="28"/>
@@ -6944,11 +6970,11 @@
       <c r="B60" s="27"/>
       <c r="C60" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.73919820499471112</v>
+        <v>-1.1489332789754789</v>
       </c>
       <c r="D60" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>1.5420015712900141</v>
+        <v>0.39778337328703695</v>
       </c>
       <c r="E60" s="36"/>
       <c r="F60" s="56" t="s">
@@ -7010,11 +7036,11 @@
       <c r="B61" s="27"/>
       <c r="C61" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-2.1625285516616732</v>
+        <v>-0.37921150971926404</v>
       </c>
       <c r="D61" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>3.9622255099924839</v>
+        <v>1.3331490414972231</v>
       </c>
       <c r="E61" s="36"/>
       <c r="F61" s="28"/>
@@ -7074,11 +7100,11 @@
       <c r="B62" s="27"/>
       <c r="C62" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>2.0712138834805311</v>
+        <v>-0.64802739265886722</v>
       </c>
       <c r="D62" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.2067408433284934</v>
+        <v>1.7725585641444626</v>
       </c>
       <c r="E62" s="36"/>
       <c r="F62" s="52" t="s">
@@ -7144,11 +7170,11 @@
       <c r="B63" s="27"/>
       <c r="C63" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.0196296050617115</v>
+        <v>1.3478590112842337</v>
       </c>
       <c r="D63" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>2.4194965826544408</v>
+        <v>1.9914071355989689</v>
       </c>
       <c r="E63" s="36"/>
       <c r="F63" s="28"/>
@@ -7208,11 +7234,11 @@
       <c r="B64" s="27"/>
       <c r="C64" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.4879718667027961</v>
+        <v>0.67776099984601912</v>
       </c>
       <c r="D64" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>1.6890011777665519</v>
+        <v>3.2842288900925025</v>
       </c>
       <c r="E64" s="36"/>
       <c r="F64" s="44" t="s">
@@ -7228,7 +7254,7 @@
       <c r="L64" s="28"/>
       <c r="M64" s="46">
         <f ca="1">ABS(G65-G70)</f>
-        <v>0.16217814826438878</v>
+        <v>0.24812140399596552</v>
       </c>
       <c r="N64" s="28"/>
       <c r="O64" s="28"/>
@@ -7285,11 +7311,11 @@
       <c r="B65" s="27"/>
       <c r="C65" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.1109504642171864</v>
+        <v>3.8920414049480115E-2</v>
       </c>
       <c r="D65" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-0.10594491975047954</v>
+        <v>1.445798361276615</v>
       </c>
       <c r="E65" s="36"/>
       <c r="F65" s="32" t="s">
@@ -7297,7 +7323,7 @@
       </c>
       <c r="G65" s="51">
         <f ca="1">AVERAGE(XOne)</f>
-        <v>-1.5552308157788439E-2</v>
+        <v>4.5842519653372264E-2</v>
       </c>
       <c r="H65" s="28"/>
       <c r="I65" s="28"/>
@@ -7308,28 +7334,28 @@
       <c r="L65" s="28"/>
       <c r="M65" s="47">
         <f ca="1">SQRT((G66^2/G67+G71^2/G72))</f>
-        <v>0.19179016621122028</v>
+        <v>0.1888092019902069</v>
       </c>
       <c r="N65" s="28"/>
       <c r="O65" s="28"/>
       <c r="P65" s="28"/>
       <c r="Q65" s="50">
-        <f ca="1">-1*M68</f>
-        <v>-1.9714346585202402</v>
+        <f ca="1">-1*M73</f>
+        <v>-1.9726626923813055</v>
       </c>
       <c r="R65" s="34" t="s">
         <v>20</v>
       </c>
       <c r="S65" s="50">
-        <f ca="1">M67</f>
-        <v>0.84560200070831837</v>
+        <f ca="1">M72</f>
+        <v>1.3141383014204733</v>
       </c>
       <c r="T65" s="34" t="s">
         <v>20</v>
       </c>
       <c r="U65" s="50">
-        <f ca="1">M68</f>
-        <v>1.9714346585202402</v>
+        <f ca="1">M73</f>
+        <v>1.9726626923813055</v>
       </c>
       <c r="V65" s="29"/>
       <c r="W65" s="1"/>
@@ -7372,11 +7398,11 @@
       <c r="B66" s="27"/>
       <c r="C66" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>2.4784552322236024</v>
+        <v>1.1738090436116593</v>
       </c>
       <c r="D66" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>1.5510429852632956</v>
+        <v>-0.41688487524883011</v>
       </c>
       <c r="E66" s="36"/>
       <c r="F66" s="32" t="s">
@@ -7384,7 +7410,7 @@
       </c>
       <c r="G66" s="51">
         <f ca="1">_xlfn.STDEV.S(XOne)</f>
-        <v>1.2899407616014686</v>
+        <v>1.1298032396516007</v>
       </c>
       <c r="H66" s="28"/>
       <c r="I66" s="28"/>
@@ -7441,11 +7467,11 @@
       <c r="B67" s="27"/>
       <c r="C67" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.79629239473958202</v>
+        <v>0.17736266792197153</v>
       </c>
       <c r="D67" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>0.7171810616816896</v>
+        <v>-0.92757704619712433</v>
       </c>
       <c r="E67" s="36"/>
       <c r="F67" s="32" t="s">
@@ -7458,13 +7484,12 @@
       <c r="H67" s="28"/>
       <c r="I67" s="28"/>
       <c r="J67" s="28"/>
-      <c r="K67" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="L67" s="28"/>
-      <c r="M67" s="46">
-        <f ca="1">M64/M65</f>
-        <v>0.84560200070831837</v>
+      <c r="K67" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="M67" s="69">
+        <f ca="1">G71^2/G66^2</f>
+        <v>1.9324457131341586</v>
       </c>
       <c r="N67" s="28"/>
       <c r="O67" s="28"/>
@@ -7518,11 +7543,11 @@
       <c r="B68" s="27"/>
       <c r="C68" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.47787485638598265</v>
+        <v>-3.7568783437819473</v>
       </c>
       <c r="D68" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-0.3584861869132735</v>
+        <v>-0.55819631500122879</v>
       </c>
       <c r="E68" s="36"/>
       <c r="F68" s="28"/>
@@ -7530,16 +7555,20 @@
       <c r="H68" s="28"/>
       <c r="I68" s="28"/>
       <c r="J68" s="28"/>
-      <c r="K68" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="L68" s="28"/>
-      <c r="M68" s="47">
-        <f ca="1">_xlfn.T.INV.2T(G77,(G67+G72-2))</f>
-        <v>1.9714346585202402</v>
-      </c>
-      <c r="N68" s="28"/>
-      <c r="O68" s="28"/>
+      <c r="K68" s="68" t="s">
+        <v>38</v>
+      </c>
+      <c r="M68" s="71">
+        <f ca="1">(1/G67+M67/G72)^2</f>
+        <v>7.7997622317268979E-4</v>
+      </c>
+      <c r="N68" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O68" s="67">
+        <f ca="1">M68/M69</f>
+        <v>188.9005694698231</v>
+      </c>
       <c r="P68" s="28"/>
       <c r="Q68" s="28"/>
       <c r="R68" s="28"/>
@@ -7587,11 +7616,11 @@
       <c r="B69" s="27"/>
       <c r="C69" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.8618834422945467</v>
+        <v>0.67974392244114479</v>
       </c>
       <c r="D69" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>0.37371249097114717</v>
+        <v>1.8143365367533884</v>
       </c>
       <c r="E69" s="36"/>
       <c r="F69" s="44" t="s">
@@ -7601,9 +7630,10 @@
       <c r="H69" s="28"/>
       <c r="I69" s="28"/>
       <c r="J69" s="28"/>
-      <c r="K69" s="28"/>
-      <c r="L69" s="28"/>
-      <c r="M69" s="28"/>
+      <c r="M69" s="72">
+        <f ca="1">1/(G67^2*(G67-1))+M67^2/(G72^2*(G72-1))</f>
+        <v>4.1290305548670732E-6</v>
+      </c>
       <c r="N69" s="28"/>
       <c r="O69" s="28"/>
       <c r="P69" s="28"/>
@@ -7653,11 +7683,11 @@
       <c r="B70" s="27"/>
       <c r="C70" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.2502107777033899</v>
+        <v>-1.2881041898124908</v>
       </c>
       <c r="D70" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.1528615262187616</v>
+        <v>0.2950005709013358</v>
       </c>
       <c r="E70" s="36"/>
       <c r="F70" s="32" t="s">
@@ -7665,14 +7695,11 @@
       </c>
       <c r="G70" s="46">
         <f ca="1">AVERAGE(XTwo)</f>
-        <v>-0.17773045642217722</v>
+        <v>-0.20227888434259325</v>
       </c>
       <c r="H70" s="28"/>
       <c r="I70" s="28"/>
       <c r="J70" s="28"/>
-      <c r="K70" s="28"/>
-      <c r="L70" s="28"/>
-      <c r="M70" s="28"/>
       <c r="N70" s="28"/>
       <c r="O70" s="28"/>
       <c r="P70" s="28"/>
@@ -7717,16 +7744,16 @@
       <c r="BC70" s="1"/>
       <c r="BD70" s="1"/>
     </row>
-    <row r="71" spans="1:56" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:56" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="27"/>
       <c r="C71" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>2.4025453436995421</v>
+        <v>2.1511194612462661</v>
       </c>
       <c r="D71" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.2872638652591815</v>
+        <v>0.71198019958362813</v>
       </c>
       <c r="E71" s="36"/>
       <c r="F71" s="32" t="s">
@@ -7734,7 +7761,7 @@
       </c>
       <c r="G71" s="51">
         <f ca="1">_xlfn.STDEV.S(XTwo)</f>
-        <v>1.4826722349758932</v>
+        <v>1.5705669960468149</v>
       </c>
       <c r="H71" s="28"/>
       <c r="I71" s="28"/>
@@ -7791,11 +7818,11 @@
       <c r="B72" s="27"/>
       <c r="C72" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-1.0230301603782452</v>
+        <v>-1.3301332043051031</v>
       </c>
       <c r="D72" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-0.36181758297803701</v>
+        <v>-0.29754317060606278</v>
       </c>
       <c r="E72" s="36"/>
       <c r="F72" s="32" t="s">
@@ -7808,9 +7835,14 @@
       <c r="H72" s="28"/>
       <c r="I72" s="28"/>
       <c r="J72" s="28"/>
-      <c r="K72" s="28"/>
+      <c r="K72" s="28" t="s">
+        <v>17</v>
+      </c>
       <c r="L72" s="28"/>
-      <c r="M72" s="28"/>
+      <c r="M72" s="46">
+        <f ca="1">M64/M65</f>
+        <v>1.3141383014204733</v>
+      </c>
       <c r="N72" s="28"/>
       <c r="O72" s="28"/>
       <c r="P72" s="28"/>
@@ -7855,16 +7887,16 @@
       <c r="BC72" s="1"/>
       <c r="BD72" s="1"/>
     </row>
-    <row r="73" spans="1:56" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:56" s="5" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="1"/>
       <c r="B73" s="27"/>
       <c r="C73" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.16866835059765267</v>
+        <v>-0.37497549465206104</v>
       </c>
       <c r="D73" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.7981967938821712</v>
+        <v>-1.3708556919929598</v>
       </c>
       <c r="E73" s="36"/>
       <c r="F73" s="28"/>
@@ -7872,9 +7904,14 @@
       <c r="H73" s="28"/>
       <c r="I73" s="28"/>
       <c r="J73" s="28"/>
-      <c r="K73" s="28"/>
+      <c r="K73" s="28" t="s">
+        <v>18</v>
+      </c>
       <c r="L73" s="28"/>
-      <c r="M73" s="28"/>
+      <c r="M73" s="47">
+        <f ca="1">_xlfn.T.INV.2T(G77,O68)</f>
+        <v>1.9726626923813055</v>
+      </c>
       <c r="N73" s="28"/>
       <c r="O73" s="28"/>
       <c r="P73" s="28"/>
@@ -7924,11 +7961,11 @@
       <c r="B74" s="27"/>
       <c r="C74" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>1.2434044707977114</v>
+        <v>-1.3068147094448521E-2</v>
       </c>
       <c r="D74" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-0.53786649249596119</v>
+        <v>-0.17060833759773308</v>
       </c>
       <c r="E74" s="36"/>
       <c r="F74" s="28"/>
@@ -7988,11 +8025,11 @@
       <c r="B75" s="27"/>
       <c r="C75" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.79634425909212914</v>
+        <v>-1.4940469373018614</v>
       </c>
       <c r="D75" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>0.60798962897531406</v>
+        <v>-1.5807104288723632</v>
       </c>
       <c r="E75" s="36"/>
       <c r="F75" s="55" t="s">
@@ -8056,11 +8093,11 @@
       <c r="B76" s="27"/>
       <c r="C76" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.44418707093657578</v>
+        <v>-0.26891460963769165</v>
       </c>
       <c r="D76" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>0.97409839195567327</v>
+        <v>-2.291295906142846</v>
       </c>
       <c r="E76" s="36"/>
       <c r="F76" s="28"/>
@@ -8120,11 +8157,11 @@
       <c r="B77" s="27"/>
       <c r="C77" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.13487078923618245</v>
+        <v>1.520406035923715</v>
       </c>
       <c r="D77" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>1.1698520581581455</v>
+        <v>-0.54640341761710121</v>
       </c>
       <c r="E77" s="36"/>
       <c r="F77" s="28" t="s">
@@ -8145,9 +8182,9 @@
       <c r="Q77" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="R77" s="57">
-        <f ca="1">_xlfn.T.DIST.2T(M67,(G67+G72-2))</f>
-        <v>0.39874649903910708</v>
+      <c r="R77" s="70">
+        <f ca="1">_xlfn.T.DIST.2T(M72,(G67+G72-2))</f>
+        <v>0.19024706136076203</v>
       </c>
       <c r="S77" s="49"/>
       <c r="T77" s="30"/>
@@ -8193,11 +8230,11 @@
       <c r="B78" s="27"/>
       <c r="C78" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.78515595871068289</v>
+        <v>0.62680241052507668</v>
       </c>
       <c r="D78" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.1575786521691398</v>
+        <v>0.68875495995998881</v>
       </c>
       <c r="E78" s="36"/>
       <c r="F78" s="28"/>
@@ -8257,11 +8294,11 @@
       <c r="B79" s="27"/>
       <c r="C79" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>0.34258246597212832</v>
+        <v>1.4444233253751353</v>
       </c>
       <c r="D79" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-0.33204502543334213</v>
+        <v>1.4551341020678747</v>
       </c>
       <c r="E79" s="36"/>
       <c r="F79" s="28"/>
@@ -8321,11 +8358,11 @@
       <c r="B80" s="27"/>
       <c r="C80" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>1.8988382652837021</v>
+        <v>1.3498881176056856</v>
       </c>
       <c r="D80" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>3.1420103061346341</v>
+        <v>-0.7311893565941654</v>
       </c>
       <c r="E80" s="36"/>
       <c r="F80" s="28"/>
@@ -8385,11 +8422,11 @@
       <c r="B81" s="27"/>
       <c r="C81" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-3.2472665298103993</v>
+        <v>0.73876640916120229</v>
       </c>
       <c r="D81" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>2.4717786042795158</v>
+        <v>-1.8763788476297965</v>
       </c>
       <c r="E81" s="36"/>
       <c r="G81" s="28"/>
@@ -8448,11 +8485,11 @@
       <c r="B82" s="27"/>
       <c r="C82" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>-0.79148992436551924</v>
+        <v>-1.1386264066169973</v>
       </c>
       <c r="D82" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-1.3105014509991495</v>
+        <v>2.5786438448305513</v>
       </c>
       <c r="E82" s="36"/>
       <c r="G82" s="28"/>
@@ -8511,11 +8548,11 @@
       <c r="B83" s="27"/>
       <c r="C83" s="36">
         <f t="shared" ca="1" si="10"/>
-        <v>1.1913484696840795</v>
+        <v>3.2689785084292947E-2</v>
       </c>
       <c r="D83" s="36">
         <f t="shared" ca="1" si="11"/>
-        <v>-0.67838269806348128</v>
+        <v>1.1184736139766089</v>
       </c>
       <c r="E83" s="36"/>
       <c r="F83" s="28"/>
@@ -8575,11 +8612,11 @@
       <c r="B84" s="27"/>
       <c r="C84" s="36">
         <f t="shared" ref="C84:C115" ca="1" si="12">_xlfn.NORM.INV(RAND(),$D$11,$D$12)</f>
-        <v>-0.55723392843134045</v>
+        <v>-1.8079962330987678</v>
       </c>
       <c r="D84" s="36">
         <f t="shared" ref="D84:D115" ca="1" si="13">_xlfn.NORM.INV(RAND(),$D$15,$D$16)</f>
-        <v>0.68883133135439345</v>
+        <v>-0.41634973484232174</v>
       </c>
       <c r="E84" s="36"/>
       <c r="F84" s="28"/>
@@ -8639,11 +8676,11 @@
       <c r="B85" s="27"/>
       <c r="C85" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.68318820226450461</v>
+        <v>3.2065702452169584</v>
       </c>
       <c r="D85" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>1.284492296705857</v>
+        <v>1.7721056899458225</v>
       </c>
       <c r="E85" s="36"/>
       <c r="F85" s="28"/>
@@ -8703,11 +8740,11 @@
       <c r="B86" s="27"/>
       <c r="C86" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.15552395300854815</v>
+        <v>0.95858410566850305</v>
       </c>
       <c r="D86" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.5230838615507751</v>
+        <v>0.57045409325809204</v>
       </c>
       <c r="E86" s="36"/>
       <c r="F86" s="28"/>
@@ -8769,11 +8806,11 @@
       <c r="B87" s="27"/>
       <c r="C87" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.8952209000857968</v>
+        <v>0.65998122380249458</v>
       </c>
       <c r="D87" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>1.297566308332454</v>
+        <v>-1.2322626018921965</v>
       </c>
       <c r="E87" s="36"/>
       <c r="F87" s="28"/>
@@ -8833,11 +8870,11 @@
       <c r="B88" s="27"/>
       <c r="C88" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-1.5629378277334216</v>
+        <v>3.0833847794743261</v>
       </c>
       <c r="D88" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>0.36422490728103357</v>
+        <v>0.69726685971186475</v>
       </c>
       <c r="E88" s="36"/>
       <c r="F88" s="28"/>
@@ -8897,11 +8934,11 @@
       <c r="B89" s="27"/>
       <c r="C89" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.1354266329792126</v>
+        <v>-0.38765156638796405</v>
       </c>
       <c r="D89" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-0.87075418960153894</v>
+        <v>-1.5903149673222217</v>
       </c>
       <c r="E89" s="36"/>
       <c r="F89" s="28"/>
@@ -8961,11 +8998,11 @@
       <c r="B90" s="27"/>
       <c r="C90" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.57905792246901111</v>
+        <v>1.2970967591795635</v>
       </c>
       <c r="D90" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.6995889834419158</v>
+        <v>-1.676022794948818</v>
       </c>
       <c r="E90" s="36"/>
       <c r="G90" s="28"/>
@@ -9024,11 +9061,11 @@
       <c r="B91" s="27"/>
       <c r="C91" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.036573554920978</v>
+        <v>-0.1627667909283822</v>
       </c>
       <c r="D91" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.6318247690914589</v>
+        <v>-1.9282363703250271</v>
       </c>
       <c r="E91" s="36"/>
       <c r="G91" s="28"/>
@@ -9087,11 +9124,11 @@
       <c r="B92" s="27"/>
       <c r="C92" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-1.8505998634869958</v>
+        <v>-0.285343546295176</v>
       </c>
       <c r="D92" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>0.56158038721881209</v>
+        <v>-1.6988410004248129</v>
       </c>
       <c r="E92" s="36"/>
       <c r="F92" s="28"/>
@@ -9151,11 +9188,11 @@
       <c r="B93" s="27"/>
       <c r="C93" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-1.4133396424977667</v>
+        <v>0.75616859706932826</v>
       </c>
       <c r="D93" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.1494926393715055</v>
+        <v>-2.1558137442313288</v>
       </c>
       <c r="E93" s="36"/>
       <c r="F93" s="28"/>
@@ -9215,11 +9252,11 @@
       <c r="B94" s="27"/>
       <c r="C94" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.61903083918157853</v>
+        <v>0.19321176404915158</v>
       </c>
       <c r="D94" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.6725965708517525</v>
+        <v>-1.2401375011291775</v>
       </c>
       <c r="E94" s="36"/>
       <c r="F94" s="28"/>
@@ -9279,11 +9316,11 @@
       <c r="B95" s="27"/>
       <c r="C95" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.4158201198402598</v>
+        <v>-0.30798466724953577</v>
       </c>
       <c r="D95" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-0.70474626833945286</v>
+        <v>-1.6723421546220034</v>
       </c>
       <c r="E95" s="36"/>
       <c r="F95" s="28"/>
@@ -9343,11 +9380,11 @@
       <c r="B96" s="27"/>
       <c r="C96" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.50732486389887899</v>
+        <v>1.0603460901595434</v>
       </c>
       <c r="D96" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-3.2911080494212315</v>
+        <v>-0.72496092213106555</v>
       </c>
       <c r="E96" s="36"/>
       <c r="F96" s="28"/>
@@ -9407,11 +9444,11 @@
       <c r="B97" s="27"/>
       <c r="C97" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.1891730324052803</v>
+        <v>0.70167139008497059</v>
       </c>
       <c r="D97" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-0.43972667867311122</v>
+        <v>0.55781567658236941</v>
       </c>
       <c r="E97" s="36"/>
       <c r="F97" s="28"/>
@@ -9471,11 +9508,11 @@
       <c r="B98" s="27"/>
       <c r="C98" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.83669639880863234</v>
+        <v>0.60223597670949036</v>
       </c>
       <c r="D98" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-0.141892926951598</v>
+        <v>0.50794668139294052</v>
       </c>
       <c r="E98" s="36"/>
       <c r="F98" s="28"/>
@@ -9535,11 +9572,11 @@
       <c r="B99" s="27"/>
       <c r="C99" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-2.2799041801092108</v>
+        <v>2.0011072099613245</v>
       </c>
       <c r="D99" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>0.74101782875146305</v>
+        <v>0.80165124455543102</v>
       </c>
       <c r="E99" s="36"/>
       <c r="F99" s="28"/>
@@ -9599,11 +9636,11 @@
       <c r="B100" s="27"/>
       <c r="C100" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-1.4641579420934649</v>
+        <v>-0.81706224715436337</v>
       </c>
       <c r="D100" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.5100261723202419</v>
+        <v>3.1050608469452232</v>
       </c>
       <c r="E100" s="36"/>
       <c r="F100" s="28"/>
@@ -9663,11 +9700,11 @@
       <c r="B101" s="27"/>
       <c r="C101" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.65956380048628438</v>
+        <v>0.14816218034037101</v>
       </c>
       <c r="D101" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>2.7487398509154666E-2</v>
+        <v>1.0157153997280084</v>
       </c>
       <c r="E101" s="36"/>
       <c r="F101" s="28"/>
@@ -9727,11 +9764,11 @@
       <c r="B102" s="27"/>
       <c r="C102" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.1036534151650028</v>
+        <v>-0.18100635489301636</v>
       </c>
       <c r="D102" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.2342761091373982</v>
+        <v>0.79138552055723099</v>
       </c>
       <c r="E102" s="36"/>
       <c r="F102" s="28"/>
@@ -9791,11 +9828,11 @@
       <c r="B103" s="27"/>
       <c r="C103" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-1.4769854389250592</v>
+        <v>0.75069616896091618</v>
       </c>
       <c r="D103" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.3005174026865607</v>
+        <v>1.0641148865701531</v>
       </c>
       <c r="E103" s="36"/>
       <c r="F103" s="28"/>
@@ -9855,11 +9892,11 @@
       <c r="B104" s="27"/>
       <c r="C104" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>2.4716263990830241</v>
+        <v>-1.2140635948103462</v>
       </c>
       <c r="D104" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>0.17200716200609617</v>
+        <v>-2.0206136829094041</v>
       </c>
       <c r="E104" s="36"/>
       <c r="F104" s="28"/>
@@ -9919,11 +9956,11 @@
       <c r="B105" s="27"/>
       <c r="C105" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.46318221707627466</v>
+        <v>0.33887211159643366</v>
       </c>
       <c r="D105" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.1441499629167544</v>
+        <v>-2.5326714819496852</v>
       </c>
       <c r="E105" s="36"/>
       <c r="F105" s="28"/>
@@ -9983,11 +10020,11 @@
       <c r="B106" s="27"/>
       <c r="C106" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.7531570074950156</v>
+        <v>1.3615321496980173</v>
       </c>
       <c r="D106" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.083702980941919</v>
+        <v>0.6864168914965727</v>
       </c>
       <c r="E106" s="36"/>
       <c r="F106" s="28"/>
@@ -10047,11 +10084,11 @@
       <c r="B107" s="27"/>
       <c r="C107" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.2948080079074345</v>
+        <v>-0.63983001613493229</v>
       </c>
       <c r="D107" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.392803738547161</v>
+        <v>0.68117503017882308</v>
       </c>
       <c r="E107" s="36"/>
       <c r="F107" s="28"/>
@@ -10111,11 +10148,11 @@
       <c r="B108" s="27"/>
       <c r="C108" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.1143374943959365</v>
+        <v>-0.6961783873451669</v>
       </c>
       <c r="D108" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-1.7570932674474882</v>
+        <v>-0.37411974442701235</v>
       </c>
       <c r="E108" s="36"/>
       <c r="F108" s="28"/>
@@ -10175,11 +10212,11 @@
       <c r="B109" s="27"/>
       <c r="C109" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.41713343618415</v>
+        <v>-0.13637403918902175</v>
       </c>
       <c r="D109" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-0.70771454381468402</v>
+        <v>-2.59692331739544</v>
       </c>
       <c r="E109" s="36"/>
       <c r="F109" s="28"/>
@@ -10239,11 +10276,11 @@
       <c r="B110" s="27"/>
       <c r="C110" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.3177378431475727</v>
+        <v>-0.90809516116592026</v>
       </c>
       <c r="D110" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>2.5913994430149074</v>
+        <v>-0.7374893565440529</v>
       </c>
       <c r="E110" s="36"/>
       <c r="F110" s="28"/>
@@ -10303,11 +10340,11 @@
       <c r="B111" s="27"/>
       <c r="C111" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>1.6761422870506357</v>
+        <v>0.19185505083543403</v>
       </c>
       <c r="D111" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-0.52430845790738345</v>
+        <v>-0.38710146729320805</v>
       </c>
       <c r="E111" s="36"/>
       <c r="F111" s="28"/>
@@ -10367,11 +10404,11 @@
       <c r="B112" s="27"/>
       <c r="C112" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-1.1250882250455825</v>
+        <v>-0.69051295784438482</v>
       </c>
       <c r="D112" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-2.9427551936363745</v>
+        <v>-0.36956149971353636</v>
       </c>
       <c r="E112" s="36"/>
       <c r="F112" s="28"/>
@@ -10431,11 +10468,11 @@
       <c r="B113" s="27"/>
       <c r="C113" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-0.61951800758083964</v>
+        <v>-0.13310794057799358</v>
       </c>
       <c r="D113" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>-0.30287823185786439</v>
+        <v>1.3055939140832638</v>
       </c>
       <c r="E113" s="36"/>
       <c r="F113" s="28"/>
@@ -10495,11 +10532,11 @@
       <c r="B114" s="27"/>
       <c r="C114" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>-1.0309125387268678</v>
+        <v>0.15318536360258964</v>
       </c>
       <c r="D114" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>1.4215748103851085</v>
+        <v>-0.93012112033894356</v>
       </c>
       <c r="E114" s="36"/>
       <c r="F114" s="28"/>
@@ -10559,11 +10596,11 @@
       <c r="B115" s="27"/>
       <c r="C115" s="36">
         <f t="shared" ca="1" si="12"/>
-        <v>0.73393397799490334</v>
+        <v>0.38417763847766107</v>
       </c>
       <c r="D115" s="36">
         <f t="shared" ca="1" si="13"/>
-        <v>8.2148079099587643E-2</v>
+        <v>-0.98086590226532411</v>
       </c>
       <c r="E115" s="36"/>
       <c r="F115" s="28"/>
@@ -10623,11 +10660,11 @@
       <c r="B116" s="27"/>
       <c r="C116" s="36">
         <f t="shared" ref="C116:C124" ca="1" si="14">_xlfn.NORM.INV(RAND(),$D$11,$D$12)</f>
-        <v>-0.91443826025031705</v>
+        <v>-0.1495823783346617</v>
       </c>
       <c r="D116" s="36">
         <f t="shared" ref="D116:D124" ca="1" si="15">_xlfn.NORM.INV(RAND(),$D$15,$D$16)</f>
-        <v>-3.5263532339540009</v>
+        <v>0.38265774615480092</v>
       </c>
       <c r="E116" s="36"/>
       <c r="F116" s="28"/>
@@ -10687,11 +10724,11 @@
       <c r="B117" s="27"/>
       <c r="C117" s="36">
         <f t="shared" ca="1" si="14"/>
-        <v>-0.59433513517905656</v>
+        <v>9.4199664376248216E-2</v>
       </c>
       <c r="D117" s="36">
         <f t="shared" ca="1" si="15"/>
-        <v>1.0356037463036882</v>
+        <v>-1.7904185706877622</v>
       </c>
       <c r="E117" s="36"/>
       <c r="F117" s="28"/>
@@ -10751,11 +10788,11 @@
       <c r="B118" s="27"/>
       <c r="C118" s="36">
         <f t="shared" ca="1" si="14"/>
-        <v>0.5842658459222988</v>
+        <v>-1.5423792627204955</v>
       </c>
       <c r="D118" s="36">
         <f t="shared" ca="1" si="15"/>
-        <v>1.1843219199114006</v>
+        <v>-0.53117745416262108</v>
       </c>
       <c r="E118" s="36"/>
       <c r="F118" s="28"/>
@@ -10815,11 +10852,11 @@
       <c r="B119" s="27"/>
       <c r="C119" s="36">
         <f t="shared" ca="1" si="14"/>
-        <v>0.76251432799380825</v>
+        <v>-0.87732041653558701</v>
       </c>
       <c r="D119" s="36">
         <f t="shared" ca="1" si="15"/>
-        <v>-0.96462606161282682</v>
+        <v>0.29619427644874452</v>
       </c>
       <c r="E119" s="36"/>
       <c r="F119" s="28"/>
@@ -10879,11 +10916,11 @@
       <c r="B120" s="27"/>
       <c r="C120" s="36">
         <f t="shared" ca="1" si="14"/>
-        <v>0.1481228370403328</v>
+        <v>-1.4344149894659275</v>
       </c>
       <c r="D120" s="36">
         <f t="shared" ca="1" si="15"/>
-        <v>-1.6751887925242404</v>
+        <v>-1.666645132918215</v>
       </c>
       <c r="E120" s="36"/>
       <c r="F120" s="28"/>
@@ -10943,11 +10980,11 @@
       <c r="B121" s="27"/>
       <c r="C121" s="36">
         <f t="shared" ca="1" si="14"/>
-        <v>-0.73490101292911525</v>
+        <v>0.707527018238848</v>
       </c>
       <c r="D121" s="36">
         <f t="shared" ca="1" si="15"/>
-        <v>0.82196625051487315</v>
+        <v>-0.59064085930563093</v>
       </c>
       <c r="E121" s="36"/>
       <c r="F121" s="28"/>
@@ -11007,11 +11044,11 @@
       <c r="B122" s="27"/>
       <c r="C122" s="36">
         <f t="shared" ca="1" si="14"/>
-        <v>-1.1226098042993955</v>
+        <v>-0.88235680133454375</v>
       </c>
       <c r="D122" s="36">
         <f t="shared" ca="1" si="15"/>
-        <v>-2.176455950021801</v>
+        <v>-4.6131363481758925</v>
       </c>
       <c r="E122" s="36"/>
       <c r="F122" s="35" t="s">
@@ -11039,11 +11076,11 @@
       <c r="B123" s="27"/>
       <c r="C123" s="36">
         <f t="shared" ca="1" si="14"/>
-        <v>-0.90937709871632488</v>
+        <v>0.14201878660582848</v>
       </c>
       <c r="D123" s="36">
         <f t="shared" ca="1" si="15"/>
-        <v>-2.1785587357213374</v>
+        <v>-0.19881796018614331</v>
       </c>
       <c r="E123" s="36"/>
       <c r="F123" s="35" t="s">
@@ -11071,11 +11108,11 @@
       <c r="B124" s="38"/>
       <c r="C124" s="6">
         <f t="shared" ca="1" si="14"/>
-        <v>-0.58466574850713193</v>
+        <v>1.444876012334672</v>
       </c>
       <c r="D124" s="6">
         <f t="shared" ca="1" si="15"/>
-        <v>2.1911585810579193</v>
+        <v>-2.1749515947598299</v>
       </c>
       <c r="E124" s="6"/>
       <c r="F124" s="39"/>

</xml_diff>